<commit_message>
removed s from zscores - typo
</commit_message>
<xml_diff>
--- a/validation/all_data.xlsx
+++ b/validation/all_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/Documents/systems-bio-research/indigo/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/Documents/systems-bio-research/INDIGO/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7002803-46A3-614E-8554-9EB0E8B08326}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C21AF17B-EB16-F84F-B76B-A3EC5E6B81B8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{CB1295CB-2541-354E-BA41-5406A90DA179}"/>
   </bookViews>
@@ -804,7 +804,7 @@
   <dimension ref="A1:AA28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -887,83 +887,83 @@
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" s="5">
-        <v>238</v>
+        <v>35</v>
+      </c>
+      <c r="B2">
+        <v>171</v>
       </c>
       <c r="C2">
-        <v>-0.15</v>
+        <v>-0.25</v>
       </c>
       <c r="D2">
-        <v>0.14000000000000001</v>
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>59</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>88</v>
+        <v>85</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>100</v>
       </c>
       <c r="L2" t="s">
         <v>18</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="N2">
-        <v>2019</v>
-      </c>
-      <c r="O2" t="s">
-        <v>21</v>
-      </c>
+        <v>2016</v>
+      </c>
+      <c r="R2" s="2"/>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3">
-        <v>171</v>
+        <v>47</v>
+      </c>
+      <c r="B3" s="5">
+        <v>238</v>
       </c>
       <c r="C3">
-        <v>-0.25</v>
+        <v>-0.15</v>
       </c>
       <c r="D3">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G3">
         <v>1</v>
       </c>
-      <c r="F3" t="s">
-        <v>59</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="L3" t="s">
         <v>18</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="N3">
-        <v>2016</v>
-      </c>
-      <c r="R3" s="2"/>
+        <v>2019</v>
+      </c>
+      <c r="O3" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -2019,7 +2019,7 @@
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="M3" r:id="rId1" xr:uid="{73381E99-A219-054A-BE83-02FD276AC453}"/>
+    <hyperlink ref="M2" r:id="rId1" xr:uid="{73381E99-A219-054A-BE83-02FD276AC453}"/>
     <hyperlink ref="M4" r:id="rId2" xr:uid="{1B0EB473-9B6A-7C43-83B2-28AE4143A5FA}"/>
     <hyperlink ref="M5" r:id="rId3" xr:uid="{5D978157-0EC6-7443-A526-2B6ABFB8F1EA}"/>
     <hyperlink ref="M6" r:id="rId4" xr:uid="{FBF34661-0882-AD4A-BC4F-77FE7AE850FD}"/>
@@ -2036,7 +2036,7 @@
     <hyperlink ref="M17" r:id="rId15" xr:uid="{FDA296EC-2574-FC4D-B43E-9F75B55AA34E}"/>
     <hyperlink ref="M18" r:id="rId16" xr:uid="{7D117953-DE02-6B4F-9D52-A62E6872BB82}"/>
     <hyperlink ref="M19" r:id="rId17" xr:uid="{C4767DEF-15D5-B940-96F1-6756FAD2C2F1}"/>
-    <hyperlink ref="M2" r:id="rId18" xr:uid="{EC2F3EBB-A2A3-0547-B976-6228FC2141C5}"/>
+    <hyperlink ref="M3" r:id="rId18" xr:uid="{EC2F3EBB-A2A3-0547-B976-6228FC2141C5}"/>
     <hyperlink ref="M20" r:id="rId19" xr:uid="{0D03EC25-6C13-C142-97C9-32E92D26F91A}"/>
     <hyperlink ref="M21" r:id="rId20" xr:uid="{4361BC35-F871-5048-BFBD-82A15D33DFF3}"/>
   </hyperlinks>

</xml_diff>

<commit_message>
camelCase to snake_case for everything
</commit_message>
<xml_diff>
--- a/validation/all_data.xlsx
+++ b/validation/all_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/Documents/systems-bio-research/INDIGO/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/Documents/systems-bio-research/INDIGO/code/validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C21AF17B-EB16-F84F-B76B-A3EC5E6B81B8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05A716E5-4949-B248-A94A-11BD4F4E33FD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{CB1295CB-2541-354E-BA41-5406A90DA179}"/>
   </bookViews>
@@ -255,15 +255,6 @@
     <t>mtb_h37rv_chandrasekaran_2016.xlsx</t>
   </si>
   <si>
-    <t>EcoliOrthologs</t>
-  </si>
-  <si>
-    <t>MtbOrthologs</t>
-  </si>
-  <si>
-    <t>PublicationYear</t>
-  </si>
-  <si>
     <t>Cutoffs are mixed but only 13 interactions, so keeping them all in one file</t>
   </si>
   <si>
@@ -288,18 +279,12 @@
     <t>m_smegmatis_nicole.xlsx</t>
   </si>
   <si>
-    <t>MtbModelExclusive</t>
-  </si>
-  <si>
     <t>mtb_yilancioglu_2019.xlsx</t>
   </si>
   <si>
     <t>mtb_h37rv_ma_2019.xlsx</t>
   </si>
   <si>
-    <t>EcoliModelExclusive</t>
-  </si>
-  <si>
     <t>Strain</t>
   </si>
   <si>
@@ -345,9 +330,6 @@
     <t>Bouvet and Grimont ATCC 17978</t>
   </si>
   <si>
-    <t>OrthologStrain</t>
-  </si>
-  <si>
     <t>Escherichia coli str. K-12 substr. MG1655</t>
   </si>
   <si>
@@ -390,7 +372,25 @@
     <t>Mycobacterium smegmatis str. MC2 155 NC_008596</t>
   </si>
   <si>
-    <t>InteractionCount</t>
+    <t>Interaction_Count</t>
+  </si>
+  <si>
+    <t>Ecoli_Orthologs</t>
+  </si>
+  <si>
+    <t>Mtb_Orthologs</t>
+  </si>
+  <si>
+    <t>Mtb_Model_Exclusive</t>
+  </si>
+  <si>
+    <t>Ecoli_Model_Exclusive</t>
+  </si>
+  <si>
+    <t>Ortholog_Strain</t>
+  </si>
+  <si>
+    <t>Publication_Year</t>
   </si>
 </sst>
 </file>
@@ -803,8 +803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{942A52AE-9ED3-674D-8E68-3209A4DF1150}">
   <dimension ref="A1:AA28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -833,7 +833,7 @@
         <v>31</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>32</v>
@@ -842,25 +842,25 @@
         <v>33</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>69</v>
+        <v>109</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>70</v>
+        <v>110</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>80</v>
+        <v>111</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>83</v>
+        <v>112</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>34</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>44</v>
@@ -869,7 +869,7 @@
         <v>28</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>71</v>
+        <v>114</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>20</v>
@@ -911,10 +911,10 @@
         <v>7</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="L2" t="s">
         <v>18</v>
@@ -950,7 +950,7 @@
         <v>14</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="L3" t="s">
         <v>18</v>
@@ -994,7 +994,7 @@
         <v>12</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="L4" t="s">
         <v>18</v>
@@ -1006,7 +1006,7 @@
         <v>2016</v>
       </c>
       <c r="O4" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="R4" s="2"/>
     </row>
@@ -1036,10 +1036,10 @@
         <v>14</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="L5" t="s">
         <v>18</v>
@@ -1078,10 +1078,10 @@
         <v>7</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="L6" t="s">
         <v>19</v>
@@ -1123,10 +1123,10 @@
         <v>7</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="K7" s="8" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="L7" t="s">
         <v>19</v>
@@ -1168,10 +1168,10 @@
         <v>17</v>
       </c>
       <c r="J8" s="8" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="L8" t="s">
         <v>19</v>
@@ -1213,10 +1213,10 @@
         <v>17</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="L9" t="s">
         <v>19</v>
@@ -1258,10 +1258,10 @@
         <v>13</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="L10" t="s">
         <v>19</v>
@@ -1303,10 +1303,10 @@
         <v>13</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="L11" t="s">
         <v>19</v>
@@ -1345,10 +1345,10 @@
         <v>7</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="K12" s="8" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="L12" t="s">
         <v>19</v>
@@ -1387,10 +1387,10 @@
         <v>7</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="K13" s="8" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="L13" t="s">
         <v>19</v>
@@ -1428,10 +1428,10 @@
         <v>7</v>
       </c>
       <c r="J14" s="8" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="K14" s="8" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="L14" t="s">
         <v>18</v>
@@ -1469,10 +1469,10 @@
         <v>7</v>
       </c>
       <c r="J15" s="8" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="K15" s="8" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="L15" t="s">
         <v>18</v>
@@ -1510,10 +1510,10 @@
         <v>7</v>
       </c>
       <c r="J16" s="8" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="K16" s="8" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="L16" t="s">
         <v>19</v>
@@ -1554,10 +1554,10 @@
         <v>7</v>
       </c>
       <c r="J17" s="8" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="K17" s="8" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="L17" t="s">
         <v>18</v>
@@ -1598,10 +1598,10 @@
         <v>11</v>
       </c>
       <c r="J18" s="8" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="K18" s="8" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="L18" t="s">
         <v>18</v>
@@ -1650,7 +1650,7 @@
     </row>
     <row r="20" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B20" s="5">
         <v>28</v>
@@ -1677,7 +1677,7 @@
         <v>29</v>
       </c>
       <c r="K20" s="8" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="L20" s="5" t="s">
         <v>18</v>
@@ -1691,7 +1691,7 @@
     </row>
     <row r="21" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B21" s="5">
         <v>71</v>
@@ -1715,10 +1715,10 @@
         <v>14</v>
       </c>
       <c r="J21" s="8" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="K21" s="8" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="L21" s="5" t="s">
         <v>18</v>
@@ -1735,7 +1735,7 @@
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B22" s="5">
         <v>10</v>
@@ -1756,7 +1756,7 @@
         <v>14</v>
       </c>
       <c r="J22" s="8" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="L22" t="s">
         <v>18</v>
@@ -1775,7 +1775,7 @@
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B23">
         <v>18</v>
@@ -1796,7 +1796,7 @@
         <v>14</v>
       </c>
       <c r="J23" s="8" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="L23" t="s">
         <v>18</v>
@@ -1811,7 +1811,7 @@
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B24">
         <v>11</v>
@@ -1832,7 +1832,7 @@
         <v>14</v>
       </c>
       <c r="J24" s="8" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="L24" t="s">
         <v>18</v>
@@ -1847,7 +1847,7 @@
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B25">
         <v>13</v>
@@ -1871,10 +1871,10 @@
         <v>14</v>
       </c>
       <c r="J25" s="8" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="K25" s="8" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="L25" t="s">
         <v>18</v>
@@ -1886,13 +1886,13 @@
         <v>29</v>
       </c>
       <c r="O25" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="T25" s="3"/>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B26">
         <v>7</v>
@@ -1919,7 +1919,7 @@
         <v>29</v>
       </c>
       <c r="K26" s="8" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="L26" t="s">
         <v>18</v>
@@ -1934,7 +1934,7 @@
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B27">
         <v>26</v>
@@ -1961,7 +1961,7 @@
         <v>29</v>
       </c>
       <c r="K27" s="8" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="L27" t="s">
         <v>18</v>
@@ -1976,7 +1976,7 @@
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B28">
         <v>20</v>
@@ -2003,7 +2003,7 @@
         <v>29</v>
       </c>
       <c r="K28" s="8" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="L28" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
removed predictor names from indigo_run
</commit_message>
<xml_diff>
--- a/validation/all_data.xlsx
+++ b/validation/all_data.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/Documents/systems-bio-research/INDIGO/code/validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DF4A825A-5D02-A84F-8F8F-2ED0985D08F9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0F40C36-97B4-5048-A890-F315990EACED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4300" yWindow="2700" windowWidth="27640" windowHeight="16940" xr2:uid="{9D1541ED-1B9A-6D45-AA86-D42E434BC003}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{9D1541ED-1B9A-6D45-AA86-D42E434BC003}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -72,9 +72,6 @@
     <t>Species</t>
   </si>
   <si>
-    <t>Strain</t>
-  </si>
-  <si>
     <t>OrtholugeDB_Strain</t>
   </si>
   <si>
@@ -136,9 +133,6 @@
   </si>
   <si>
     <t>ecoli_mg1655_chandrasekaran_2016.xlsx</t>
-  </si>
-  <si>
-    <t>E. coli MG1655  (171)</t>
   </si>
   <si>
     <t>E. coli MG1655 Chandrasekaran 2016 (171)</t>
@@ -450,22 +444,28 @@
     <t>M. tb H37Rv Ma 2019 mtb (241)</t>
   </si>
   <si>
-    <t>mtb_h37rv_nicole_mtb.xlsx</t>
-  </si>
-  <si>
     <t>M. tb H37Rv (39)</t>
   </si>
   <si>
-    <t>M. tb H37Rv Nicole mtb (39)</t>
-  </si>
-  <si>
-    <t>Nicole - multiple sources</t>
-  </si>
-  <si>
     <t>NA</t>
   </si>
   <si>
-    <t>Cutoffs are mixed but only 13 interactions, so keeping them all in one file</t>
+    <t>E. coli MG1655 (171)</t>
+  </si>
+  <si>
+    <t>mtb_h37rv_rhoads.xlsx</t>
+  </si>
+  <si>
+    <t>M. tb H37Rv Rhoads (39)</t>
+  </si>
+  <si>
+    <t>Multiple sources</t>
+  </si>
+  <si>
+    <t>Compiled by Nicole Rhoads</t>
+  </si>
+  <si>
+    <t>Strain_Subspecies</t>
   </si>
 </sst>
 </file>
@@ -883,10 +883,15 @@
   <dimension ref="A1:AB21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -926,22 +931,22 @@
         <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
@@ -958,13 +963,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" t="s">
         <v>19</v>
-      </c>
-      <c r="D2" t="s">
-        <v>20</v>
       </c>
       <c r="E2">
         <v>190</v>
@@ -976,28 +981,28 @@
         <v>0.25</v>
       </c>
       <c r="I2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" t="s">
         <v>22</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>23</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>24</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>26</v>
       </c>
       <c r="Q2" s="5">
         <v>38795</v>
@@ -1008,13 +1013,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" t="s">
         <v>28</v>
-      </c>
-      <c r="D3" t="s">
-        <v>29</v>
       </c>
       <c r="E3">
         <v>166</v>
@@ -1026,28 +1031,28 @@
         <v>0.25</v>
       </c>
       <c r="I3" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="M3" t="s">
+        <v>29</v>
+      </c>
+      <c r="N3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O3" t="s">
         <v>30</v>
       </c>
-      <c r="N3" t="s">
-        <v>24</v>
-      </c>
-      <c r="O3" t="s">
+      <c r="P3" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="P3" s="4" t="s">
-        <v>32</v>
       </c>
       <c r="Q3" s="5">
         <v>41834</v>
@@ -1058,13 +1063,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D4" t="s">
         <v>33</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" t="s">
-        <v>35</v>
       </c>
       <c r="E4">
         <v>171</v>
@@ -1076,28 +1081,28 @@
         <v>1</v>
       </c>
       <c r="I4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4" s="3" t="s">
+      <c r="M4" t="s">
         <v>22</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>23</v>
       </c>
-      <c r="N4" t="s">
-        <v>24</v>
-      </c>
       <c r="O4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P4" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="Q4" s="5">
         <v>42513</v>
@@ -1108,13 +1113,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" t="s">
         <v>37</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" t="s">
-        <v>39</v>
       </c>
       <c r="E5">
         <v>45</v>
@@ -1126,31 +1131,31 @@
         <v>1</v>
       </c>
       <c r="H5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="I5" t="s">
+      <c r="M5" t="s">
         <v>41</v>
       </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5" s="3" t="s">
+      <c r="N5" t="s">
         <v>42</v>
       </c>
-      <c r="M5" t="s">
-        <v>43</v>
-      </c>
-      <c r="N5" t="s">
-        <v>44</v>
-      </c>
       <c r="O5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P5" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="Q5" s="5">
         <v>42514</v>
@@ -1161,13 +1166,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" t="s">
         <v>45</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D6" t="s">
-        <v>47</v>
       </c>
       <c r="E6">
         <v>316</v>
@@ -1179,28 +1184,28 @@
         <v>0.1</v>
       </c>
       <c r="I6" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="M6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="N6" t="s">
+        <v>23</v>
+      </c>
+      <c r="O6" t="s">
         <v>24</v>
       </c>
-      <c r="O6" t="s">
-        <v>25</v>
-      </c>
       <c r="P6" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="Q6" s="5">
         <v>43285</v>
@@ -1211,13 +1216,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" t="s">
         <v>49</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D7" t="s">
-        <v>51</v>
       </c>
       <c r="E7">
         <v>316</v>
@@ -1229,31 +1234,31 @@
         <v>0.1</v>
       </c>
       <c r="H7" t="s">
+        <v>50</v>
+      </c>
+      <c r="I7" t="s">
+        <v>51</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="M7" t="s">
         <v>52</v>
       </c>
-      <c r="I7" t="s">
+      <c r="N7" t="s">
         <v>53</v>
       </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="M7" t="s">
-        <v>54</v>
-      </c>
-      <c r="N7" t="s">
-        <v>55</v>
-      </c>
       <c r="O7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P7" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="Q7" s="5">
         <v>43286</v>
@@ -1264,13 +1269,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" t="s">
         <v>56</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D8" t="s">
-        <v>58</v>
       </c>
       <c r="E8" s="7">
         <v>248</v>
@@ -1282,31 +1287,31 @@
         <v>0.1</v>
       </c>
       <c r="H8" t="s">
+        <v>57</v>
+      </c>
+      <c r="I8" t="s">
+        <v>58</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="I8" t="s">
+      <c r="M8" t="s">
         <v>60</v>
       </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8" s="3" t="s">
+      <c r="N8" t="s">
         <v>61</v>
       </c>
-      <c r="M8" t="s">
-        <v>62</v>
-      </c>
-      <c r="N8" t="s">
-        <v>63</v>
-      </c>
       <c r="O8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P8" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="Q8" s="5">
         <v>43287</v>
@@ -1317,13 +1322,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D9" t="s">
         <v>64</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D9" t="s">
-        <v>66</v>
       </c>
       <c r="E9" s="7">
         <v>248</v>
@@ -1335,31 +1340,31 @@
         <v>0.1</v>
       </c>
       <c r="H9" t="s">
+        <v>65</v>
+      </c>
+      <c r="I9" t="s">
+        <v>66</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="M9" t="s">
         <v>67</v>
       </c>
-      <c r="I9" t="s">
+      <c r="N9" t="s">
         <v>68</v>
       </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="M9" t="s">
-        <v>69</v>
-      </c>
-      <c r="N9" t="s">
-        <v>70</v>
-      </c>
       <c r="O9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P9" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="Q9" s="5">
         <v>43288</v>
@@ -1370,13 +1375,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D10" t="s">
         <v>71</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D10" t="s">
-        <v>73</v>
       </c>
       <c r="E10">
         <v>163</v>
@@ -1388,31 +1393,31 @@
         <v>0.1</v>
       </c>
       <c r="H10" t="s">
+        <v>72</v>
+      </c>
+      <c r="I10" t="s">
+        <v>73</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="I10" t="s">
+      <c r="M10" t="s">
         <v>75</v>
       </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10" s="3" t="s">
+      <c r="N10" t="s">
         <v>76</v>
       </c>
-      <c r="M10" t="s">
-        <v>77</v>
-      </c>
-      <c r="N10" t="s">
-        <v>78</v>
-      </c>
       <c r="O10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P10" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="Q10" s="5">
         <v>43289</v>
@@ -1423,13 +1428,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D11" t="s">
         <v>79</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D11" t="s">
-        <v>81</v>
       </c>
       <c r="E11" s="7">
         <v>163</v>
@@ -1441,31 +1446,31 @@
         <v>0.1</v>
       </c>
       <c r="H11" t="s">
+        <v>80</v>
+      </c>
+      <c r="I11" t="s">
+        <v>81</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="M11" t="s">
         <v>82</v>
       </c>
-      <c r="I11" t="s">
+      <c r="N11" t="s">
         <v>83</v>
       </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="M11" t="s">
-        <v>84</v>
-      </c>
-      <c r="N11" t="s">
-        <v>85</v>
-      </c>
       <c r="O11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P11" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="Q11" s="5">
         <v>43290</v>
@@ -1476,13 +1481,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>84</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D12" t="s">
         <v>86</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D12" t="s">
-        <v>88</v>
       </c>
       <c r="E12">
         <v>49</v>
@@ -1494,28 +1499,28 @@
         <v>0.25</v>
       </c>
       <c r="I12" t="s">
+        <v>20</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="J12">
-        <v>0</v>
-      </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
-      <c r="L12" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="M12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="N12" t="s">
+        <v>23</v>
+      </c>
+      <c r="O12" t="s">
         <v>24</v>
       </c>
-      <c r="O12" t="s">
-        <v>25</v>
-      </c>
       <c r="P12" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="Q12" s="5">
         <v>43388</v>
@@ -1526,13 +1531,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D13" t="s">
         <v>91</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D13" t="s">
-        <v>93</v>
       </c>
       <c r="E13">
         <v>49</v>
@@ -1544,28 +1549,28 @@
         <v>0.25</v>
       </c>
       <c r="I13" t="s">
+        <v>20</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="J13">
-        <v>0</v>
-      </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
-      <c r="L13" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="M13" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="N13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P13" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="Q13" s="5">
         <v>43388</v>
@@ -1576,13 +1581,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D14" t="s">
         <v>94</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D14" t="s">
-        <v>96</v>
       </c>
       <c r="E14">
         <v>180</v>
@@ -1594,34 +1599,34 @@
         <v>0.2</v>
       </c>
       <c r="I14" t="s">
+        <v>20</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="J14">
-        <v>0</v>
-      </c>
-      <c r="K14">
-        <v>0</v>
-      </c>
-      <c r="L14" s="3" t="s">
+      <c r="M14" t="s">
         <v>22</v>
       </c>
-      <c r="M14" t="s">
+      <c r="N14" t="s">
         <v>23</v>
       </c>
-      <c r="N14" t="s">
-        <v>24</v>
-      </c>
       <c r="O14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P14" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="Q14" s="5">
         <v>43465</v>
       </c>
       <c r="R14" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.2">
@@ -1629,13 +1634,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>97</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D15" t="s">
         <v>99</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D15" t="s">
-        <v>101</v>
       </c>
       <c r="E15">
         <v>45</v>
@@ -1647,37 +1652,37 @@
         <v>0.2</v>
       </c>
       <c r="H15" t="s">
+        <v>100</v>
+      </c>
+      <c r="I15" t="s">
+        <v>101</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="I15" t="s">
+      <c r="M15" t="s">
         <v>103</v>
       </c>
-      <c r="J15">
-        <v>0</v>
-      </c>
-      <c r="K15">
-        <v>0</v>
-      </c>
-      <c r="L15" s="3" t="s">
+      <c r="N15" t="s">
         <v>104</v>
       </c>
-      <c r="M15" t="s">
-        <v>105</v>
-      </c>
-      <c r="N15" t="s">
-        <v>106</v>
-      </c>
       <c r="O15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P15" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="Q15" s="5">
         <v>43465</v>
       </c>
       <c r="R15" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.2">
@@ -1685,13 +1690,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
+        <v>106</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D16" t="s">
         <v>108</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="D16" t="s">
-        <v>110</v>
       </c>
       <c r="E16">
         <v>82</v>
@@ -1703,34 +1708,34 @@
         <v>0.1</v>
       </c>
       <c r="I16" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="J16">
-        <v>0</v>
-      </c>
-      <c r="K16">
-        <v>0</v>
-      </c>
-      <c r="L16" s="3" t="s">
+      <c r="M16" t="s">
         <v>22</v>
       </c>
-      <c r="M16" t="s">
+      <c r="N16" t="s">
         <v>23</v>
       </c>
-      <c r="N16" t="s">
+      <c r="O16" t="s">
         <v>24</v>
       </c>
-      <c r="O16" t="s">
-        <v>25</v>
-      </c>
       <c r="P16" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="Q16" s="5">
         <v>43495</v>
       </c>
       <c r="R16" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.2">
@@ -1738,13 +1743,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
+        <v>111</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D17" t="s">
         <v>113</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D17" t="s">
-        <v>115</v>
       </c>
       <c r="E17">
         <v>28</v>
@@ -1756,7 +1761,7 @@
         <v>0</v>
       </c>
       <c r="H17" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="J17">
         <v>0</v>
@@ -1765,22 +1770,22 @@
         <v>1</v>
       </c>
       <c r="L17" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="N17" t="s">
+        <v>116</v>
+      </c>
+      <c r="O17" t="s">
+        <v>30</v>
+      </c>
+      <c r="P17" s="8" t="s">
         <v>117</v>
-      </c>
-      <c r="N17" t="s">
-        <v>118</v>
-      </c>
-      <c r="O17" t="s">
-        <v>31</v>
-      </c>
-      <c r="P17" s="8" t="s">
-        <v>119</v>
       </c>
       <c r="Q17" s="5">
         <v>43692</v>
       </c>
       <c r="R17" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.2">
@@ -1788,13 +1793,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
+        <v>119</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D18" t="s">
         <v>121</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D18" t="s">
-        <v>123</v>
       </c>
       <c r="E18">
         <v>120</v>
@@ -1812,19 +1817,19 @@
         <v>0</v>
       </c>
       <c r="L18" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="O18" t="s">
+        <v>30</v>
+      </c>
+      <c r="P18" s="4" t="s">
         <v>117</v>
-      </c>
-      <c r="O18" t="s">
-        <v>31</v>
-      </c>
-      <c r="P18" s="4" t="s">
-        <v>119</v>
       </c>
       <c r="Q18" s="5">
         <v>43692</v>
       </c>
       <c r="R18" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.2">
@@ -1832,13 +1837,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
+        <v>123</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D19" t="s">
         <v>125</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="D19" t="s">
-        <v>127</v>
       </c>
       <c r="E19">
         <v>74</v>
@@ -1850,7 +1855,7 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="H19" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="J19">
         <v>0</v>
@@ -1859,25 +1864,25 @@
         <v>1</v>
       </c>
       <c r="L19" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="M19" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="N19" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="O19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P19" s="8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="Q19" s="5">
         <v>43781</v>
       </c>
       <c r="R19" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.2">
@@ -1885,13 +1890,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
+        <v>129</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D20" t="s">
         <v>131</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="D20" t="s">
-        <v>133</v>
       </c>
       <c r="E20">
         <v>241</v>
@@ -1909,22 +1914,22 @@
         <v>0</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="M20" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="O20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P20" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="Q20" s="5">
         <v>43781</v>
       </c>
       <c r="R20" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.2">
@@ -1932,10 +1937,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D21" t="s">
         <v>136</v>
@@ -1950,7 +1955,7 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="H21" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="J21">
         <v>1</v>
@@ -1959,49 +1964,49 @@
         <v>0</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="M21" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="N21" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="O21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P21" t="s">
         <v>137</v>
       </c>
       <c r="Q21" t="s">
+        <v>133</v>
+      </c>
+      <c r="R21" t="s">
         <v>138</v>
-      </c>
-      <c r="R21" t="s">
-        <v>139</v>
       </c>
       <c r="U21" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="P16" r:id="rId1" xr:uid="{964A04E4-4B05-6041-8EF5-AAA6B9F8B67E}"/>
-    <hyperlink ref="P2" r:id="rId2" xr:uid="{B177441F-9F9A-AC43-926D-DFBFEF9440E0}"/>
-    <hyperlink ref="P4" r:id="rId3" xr:uid="{CD4F476E-1534-EC46-B60D-52ED431E9587}"/>
-    <hyperlink ref="P5" r:id="rId4" xr:uid="{54A258E9-FB3A-D846-A73B-0EF9B944526D}"/>
-    <hyperlink ref="P6" r:id="rId5" xr:uid="{AA62CA4F-490E-3140-9A9E-DF98FBC92053}"/>
-    <hyperlink ref="P7" r:id="rId6" xr:uid="{E393F320-AD4B-1349-B090-BA023FC476A3}"/>
-    <hyperlink ref="P8" r:id="rId7" xr:uid="{60A2D410-636F-AB46-ABFA-7F8AA330930F}"/>
-    <hyperlink ref="P9" r:id="rId8" xr:uid="{C3EF977B-705B-124D-B04C-82ACB5CDB80E}"/>
-    <hyperlink ref="P10" r:id="rId9" xr:uid="{8DADE49E-F1A4-B046-83F6-5937714C5D8D}"/>
-    <hyperlink ref="P11" r:id="rId10" xr:uid="{187F8617-AEE4-C04D-BA66-67B08FF6DD35}"/>
-    <hyperlink ref="P3" r:id="rId11" xr:uid="{A216FB09-E581-C14F-B839-ABD5D2EBCFB8}"/>
-    <hyperlink ref="P14" r:id="rId12" xr:uid="{EF54685F-0F4C-C84D-B0CF-87FA38FF12FD}"/>
-    <hyperlink ref="P15" r:id="rId13" xr:uid="{A461EFB0-8C2C-8147-9E94-68376281FEBC}"/>
-    <hyperlink ref="P18" r:id="rId14" display="Design of high-order antibiotic combinations against M. tuberculosis by ranking and exclusion, Yilancioglu et al." xr:uid="{A11342A7-588B-E241-B24E-CBCF48C92401}"/>
-    <hyperlink ref="P17" r:id="rId15" display="Design of high-order antibiotic combinations against M. tuberculosis by ranking and exclusion, Yilancioglu et al." xr:uid="{EC2F72DB-060B-8249-89C3-B2E06C2192CE}"/>
-    <hyperlink ref="P19" r:id="rId16" xr:uid="{C7FC6951-9F71-AF40-9D6B-8F7B82ADA7C1}"/>
-    <hyperlink ref="P20" r:id="rId17" xr:uid="{FCEC9EA5-BE3D-304C-AD6D-27884DD37E1C}"/>
-    <hyperlink ref="P12" r:id="rId18" display="Additivity of inhibitory effects in multidrug combinations, Russ et al." xr:uid="{BAFCBB3F-8962-7042-A4D6-1BB687B3F445}"/>
-    <hyperlink ref="P13" r:id="rId19" display="Additivity of inhibitory effects in multidrug combinations, Russ et al." xr:uid="{CA013F94-0703-0D40-B4A5-904E71B5093C}"/>
+    <hyperlink ref="P16" r:id="rId1" xr:uid="{2517B57E-5C02-9B4A-931E-2B52BA7E4767}"/>
+    <hyperlink ref="P2" r:id="rId2" xr:uid="{9516D4A8-DEC6-3245-88CB-C3C4E933A42C}"/>
+    <hyperlink ref="P4" r:id="rId3" xr:uid="{D4BA18AF-7267-D44D-808C-8F357CAB57AE}"/>
+    <hyperlink ref="P5" r:id="rId4" xr:uid="{25F97092-5552-5748-9276-0AB4DAB4EA85}"/>
+    <hyperlink ref="P6" r:id="rId5" xr:uid="{78C681D7-F91A-A744-8AE6-2F64CE077C12}"/>
+    <hyperlink ref="P7" r:id="rId6" xr:uid="{8C4E4AB2-1185-9C4D-99FA-E70F89334B35}"/>
+    <hyperlink ref="P8" r:id="rId7" xr:uid="{6EC4E5B7-D277-9445-A809-52F255CB50C9}"/>
+    <hyperlink ref="P9" r:id="rId8" xr:uid="{22FF48B5-9C1F-B647-904A-A1080FBC1D3B}"/>
+    <hyperlink ref="P10" r:id="rId9" xr:uid="{D12FE1A0-B565-DD41-8034-9CB952785638}"/>
+    <hyperlink ref="P11" r:id="rId10" xr:uid="{8C49BAAB-D33B-6345-BF80-6C8EE3D2B1AE}"/>
+    <hyperlink ref="P3" r:id="rId11" xr:uid="{1F272CE9-D725-854B-A4A8-0F5DCE6F5858}"/>
+    <hyperlink ref="P14" r:id="rId12" xr:uid="{104D0485-E5C6-F44E-8656-0CEDC7E41895}"/>
+    <hyperlink ref="P15" r:id="rId13" xr:uid="{1D669A33-C456-214E-A8B8-6BED532DADDE}"/>
+    <hyperlink ref="P18" r:id="rId14" display="Design of high-order antibiotic combinations against M. tuberculosis by ranking and exclusion, Yilancioglu et al." xr:uid="{91ED7E6D-4D78-B547-B391-101A2EEC09AD}"/>
+    <hyperlink ref="P17" r:id="rId15" display="Design of high-order antibiotic combinations against M. tuberculosis by ranking and exclusion, Yilancioglu et al." xr:uid="{654272A8-36F0-F143-8627-5756DAEB8AA2}"/>
+    <hyperlink ref="P19" r:id="rId16" xr:uid="{75E6762B-CBB2-7B42-924B-18FC85358655}"/>
+    <hyperlink ref="P20" r:id="rId17" xr:uid="{817A12DB-F5AB-9A40-B6C0-9D926F3149CA}"/>
+    <hyperlink ref="P12" r:id="rId18" display="Additivity of inhibitory effects in multidrug combinations, Russ et al." xr:uid="{B5AD60D8-29BD-7E4F-B32F-AF2F64C7C7FB}"/>
+    <hyperlink ref="P13" r:id="rId19" display="Additivity of inhibitory effects in multidrug combinations, Russ et al." xr:uid="{19704051-6A63-D343-92D8-050C701F82D4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>